<commit_message>
data is being render according to RFID
</commit_message>
<xml_diff>
--- a/frontend/src/assets/data.xlsx
+++ b/frontend/src/assets/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peerg\Desktop\rfid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peerg\Desktop\onShoes\frontend\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8AE791-E0AC-44B3-93FD-476B826AE2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73F6D62-F2B8-42AD-8A22-C4495DA0D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E70A7F8-D375-46E0-BE78-AFF6D5690182}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>https://drive.google.com/file/d/1Qfoaa7mGEVmrpEoKmsHOmgQnVUhh755V/view?usp=drivesdk1Qfoaa7mGEVmrpEoKmsHOmgQnVUhh755V</t>
   </si>
@@ -182,28 +182,19 @@
     <t>activity</t>
   </si>
   <si>
-    <t>running</t>
-  </si>
-  <si>
     <t>running_distance</t>
   </si>
   <si>
-    <t>road</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
     <t>https://ingsport.co.il/wp-content/uploads/2022/03/Small-PNG-59.98986-cloud_5-ss22-all_black-m-g1.png</t>
   </si>
   <si>
     <t>https://ingsport.co.il/wp-content/uploads/2022/04/59.98912-cloud_5-ss22-olive_white-m-g1-1.png</t>
   </si>
   <si>
-    <t>daily</t>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>damping</t>
   </si>
 </sst>
 </file>
@@ -680,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67BB82-E1F4-42A8-B8E4-7008364C0D33}">
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AY12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AX3" sqref="AX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,7 +688,7 @@
     <col min="12" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>39</v>
       </c>
@@ -711,7 +702,7 @@
         <v>37</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>47</v>
@@ -803,8 +794,14 @@
       <c r="AI1" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="AX1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" s="1" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" s="1" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -818,16 +815,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="I2" s="3">
         <v>820</v>
@@ -836,7 +833,7 @@
         <v>690</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -895,8 +892,14 @@
       <c r="AI2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="AX2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" s="1" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" s="1" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -910,16 +913,16 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="I3" s="3">
         <v>700</v>
@@ -928,7 +931,7 @@
         <v>590</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>3</v>
@@ -969,8 +972,14 @@
       <c r="AI3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AX3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G12" s="14"/>
     </row>
   </sheetData>

</xml_diff>